<commit_message>
Proces testet og tilrettet formattering af tekst.
</commit_message>
<xml_diff>
--- a/Regler.xlsx
+++ b/Regler.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\RPA\Leverancer\Opret digital ansøgning til personlige hjælpemidler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC3BF208-39D3-463B-9582-6E03A80E52BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A03849C-861F-4AAE-8B73-7AFEA53150CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CAA54819-A61F-4598-B5CA-D657E4BAC226}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CAA54819-A61F-4598-B5CA-D657E4BAC226}"/>
   </bookViews>
   <sheets>
     <sheet name="Opgaveansvarlig organisation" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="77">
   <si>
     <t>Hjælpemiddel</t>
   </si>
@@ -45,24 +45,12 @@
     <t>Organisation</t>
   </si>
   <si>
-    <t>Ortopdisk fodtøj</t>
-  </si>
-  <si>
     <t>Team Kropsbårne hjælpemidler</t>
   </si>
   <si>
-    <t>Diabeteshjælpemidler</t>
-  </si>
-  <si>
     <t>Sygeplejehjælpemidler</t>
   </si>
   <si>
-    <t>Skinne/bandage</t>
-  </si>
-  <si>
-    <t>Forhøjelse/tilretning af eget fodtøj</t>
-  </si>
-  <si>
     <t>Korset</t>
   </si>
   <si>
@@ -72,32 +60,221 @@
     <t>Andet</t>
   </si>
   <si>
-    <t>Kontinenshjælpemidler (bleer/katetre)</t>
-  </si>
-  <si>
-    <t>Stomihjælpemidler (inkl. stomibrokbandage)</t>
-  </si>
-  <si>
-    <t>Protese (bryst, øjne, arme og ben)</t>
-  </si>
-  <si>
-    <t>Kompressionsstrømper (f.eks.støttestrømper)</t>
-  </si>
-  <si>
-    <t>Ortopædisk fodindlæg (arm, ben, finder mm.)</t>
-  </si>
-  <si>
-    <t>Hjælpemiddel - Xflow</t>
-  </si>
-  <si>
     <t>Sagsområde - Nexus</t>
+  </si>
+  <si>
+    <t>Ortopædisk fodindlæg - Højre fod</t>
+  </si>
+  <si>
+    <t>Ortopædisk fodindlæg - Venstre fod</t>
+  </si>
+  <si>
+    <t>Ortopædisk fodindlæg - Begge fødder</t>
+  </si>
+  <si>
+    <t>Diabeteshjælpemiddel - Injektionsbehandling</t>
+  </si>
+  <si>
+    <t>Diabeteshjælpemiddel - Tabletbehandling</t>
+  </si>
+  <si>
+    <t>Kontinenshjælpemiddel - Bleer</t>
+  </si>
+  <si>
+    <t>Kontinenshjælpemiddel - Kateterprodukter</t>
+  </si>
+  <si>
+    <t>Kontinenshjælpemiddel - Uridomer</t>
+  </si>
+  <si>
+    <t>Stomihjælpemiddel</t>
+  </si>
+  <si>
+    <t>Stomihjælpemiddel - Stomibrokbandage eller -bælte</t>
+  </si>
+  <si>
+    <t>Protese - Arm</t>
+  </si>
+  <si>
+    <t>Protese - Ben</t>
+  </si>
+  <si>
+    <t>Protese - Bryst</t>
+  </si>
+  <si>
+    <t>Protese - Øjen</t>
+  </si>
+  <si>
+    <t>Kompressionsstrømper og støttestrømper - Højre ben</t>
+  </si>
+  <si>
+    <t>Kompressionsstrømper og støttestrømper - Venstre ben</t>
+  </si>
+  <si>
+    <t>Kompressionsstrømper og støttestrømper - Begge ben</t>
+  </si>
+  <si>
+    <t>Kompressionsstrømper og støttestrømper - Højre arm</t>
+  </si>
+  <si>
+    <t>Kompressionsstrømper og støttestrømper - Venstre arm</t>
+  </si>
+  <si>
+    <t>Kompressionsstrømper og støttestrømper - Begge arme</t>
+  </si>
+  <si>
+    <t>Kompressionsstrømper og støttestrømper - Handske</t>
+  </si>
+  <si>
+    <t>Ortopædisk fodtøj</t>
+  </si>
+  <si>
+    <t>Albueskinne - Højre arm</t>
+  </si>
+  <si>
+    <t>Albueskinne - Venstre arm</t>
+  </si>
+  <si>
+    <t>Albueskinner - Begge arme</t>
+  </si>
+  <si>
+    <t>Knæskinne - Højre knæ</t>
+  </si>
+  <si>
+    <t>Knæskinne - Venstre knæ</t>
+  </si>
+  <si>
+    <t>Knæskinner - Begge knæ</t>
+  </si>
+  <si>
+    <t>Håndledsskinne - Højre hånd</t>
+  </si>
+  <si>
+    <t>Håndledsskinne - Venstre hånd</t>
+  </si>
+  <si>
+    <t>Håndledsskinne - Begge hænder</t>
+  </si>
+  <si>
+    <t>Tommelskinne - Højre hånd</t>
+  </si>
+  <si>
+    <t>Tommelskinne - Venstre hånd</t>
+  </si>
+  <si>
+    <t>Tommelskinne - Begge hænder</t>
+  </si>
+  <si>
+    <t>Skulderskinne - Højre arm</t>
+  </si>
+  <si>
+    <t>Skulderskinne - Venstre arm</t>
+  </si>
+  <si>
+    <t>Skulderskinne - Begge arme</t>
+  </si>
+  <si>
+    <t>Ankelskinne - Højre fod</t>
+  </si>
+  <si>
+    <t>Ankelskinne - Venstre fod</t>
+  </si>
+  <si>
+    <t>Ankelskinne - Begge fødder</t>
+  </si>
+  <si>
+    <t>Halskrave</t>
+  </si>
+  <si>
+    <t>Brokbandage</t>
+  </si>
+  <si>
+    <t>Forhøjelse/tilretning af almindeligt fodtøj</t>
+  </si>
+  <si>
+    <t>Andre personlige hjælpemidler</t>
+  </si>
+  <si>
+    <t>Hånd- og benskinner</t>
+  </si>
+  <si>
+    <t>Støttekorsetter</t>
+  </si>
+  <si>
+    <t>Arm- og benproteser</t>
+  </si>
+  <si>
+    <t>Brystproteser</t>
+  </si>
+  <si>
+    <t>Optiske synshjælpemidler</t>
+  </si>
+  <si>
+    <t>Parykker</t>
+  </si>
+  <si>
+    <t>Katetre</t>
+  </si>
+  <si>
+    <t>Bleer</t>
+  </si>
+  <si>
+    <t>Stomihjælpemidler</t>
+  </si>
+  <si>
+    <t>Uridomer</t>
+  </si>
+  <si>
+    <t>Injektions- og testmaterialer</t>
+  </si>
+  <si>
+    <t>Tilretning og forhøjelse af fodtøj</t>
+  </si>
+  <si>
+    <t>Kompressionsstrømper</t>
+  </si>
+  <si>
+    <t>Ortopædisk fodtøj og indlæ</t>
+  </si>
+  <si>
+    <t>Ortopædisk fodindlæg</t>
+  </si>
+  <si>
+    <t>Kontinenshjælpemiddel</t>
+  </si>
+  <si>
+    <t>Protese</t>
+  </si>
+  <si>
+    <t>Kompressionsstrømper og støttestrømper</t>
+  </si>
+  <si>
+    <t>Albueskinne</t>
+  </si>
+  <si>
+    <t>Knæskinne</t>
+  </si>
+  <si>
+    <t>Håndledsskinne</t>
+  </si>
+  <si>
+    <t>Tommelskinne</t>
+  </si>
+  <si>
+    <t>Skulderskinne</t>
+  </si>
+  <si>
+    <t>Ankelskinne</t>
+  </si>
+  <si>
+    <t>Hjælpemiddel - XFlow</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,6 +293,19 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -150,10 +340,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,15 +680,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01B23E15-DB25-4893-BDEE-BEC2579ACCDF}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="A20" sqref="A20:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.5703125" customWidth="1"/>
+    <col min="1" max="1" width="52.5703125" customWidth="1"/>
     <col min="2" max="2" width="52.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -509,99 +701,147 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
+      <c r="A2" t="s">
+        <v>66</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
+      <c r="A3" t="s">
+        <v>67</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>11</v>
+      <c r="A4" t="s">
+        <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="B18" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>3</v>
+      <c r="B19" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -611,24 +851,398 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA2CB316-3EF2-470C-97ED-F33EF84A885D}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" customWidth="1"/>
+    <col min="1" max="1" width="53.7109375" customWidth="1"/>
     <col min="2" max="2" width="41.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>47</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>50</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>